<commit_message>
add some code for compare with fe, without fe and fe+ smothe
</commit_message>
<xml_diff>
--- a/rill_final_enhanced/comprehensive_results.xlsx
+++ b/rill_final_enhanced/comprehensive_results.xlsx
@@ -12,13 +12,14 @@
     <sheet name="Feature_Importance" sheetId="3" r:id="rId3"/>
     <sheet name="Hyperparameter_Tuning" sheetId="4" r:id="rId4"/>
     <sheet name="Summary" sheetId="5" r:id="rId5"/>
+    <sheet name="Comparative_Results" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="89">
   <si>
     <t>Model</t>
   </si>
@@ -41,12 +42,12 @@
     <t>XGBoost</t>
   </si>
   <si>
+    <t>GBM</t>
+  </si>
+  <si>
     <t>LightGBM</t>
   </si>
   <si>
-    <t>GBM</t>
-  </si>
-  <si>
     <t>RandomForest</t>
   </si>
   <si>
@@ -95,52 +96,55 @@
     <t>Contract_Two year</t>
   </si>
   <si>
+    <t>Churn_Risk_Score</t>
+  </si>
+  <si>
+    <t>PaperlessBilling_Yes</t>
+  </si>
+  <si>
     <t>PaymentMethod_Electronic check</t>
   </si>
   <si>
-    <t>PaperlessBilling_Yes</t>
-  </si>
-  <si>
-    <t>Churn_Risk_Score</t>
+    <t>Contract_One year</t>
+  </si>
+  <si>
+    <t>TechSupport_Yes</t>
   </si>
   <si>
     <t>gender_Male</t>
   </si>
   <si>
-    <t>Contract_One year</t>
-  </si>
-  <si>
     <t>MultipleLines_Yes</t>
   </si>
   <si>
-    <t>TechSupport_Yes</t>
+    <t>MonthlyCharges</t>
   </si>
   <si>
     <t>OnlineSecurity_Yes</t>
   </si>
   <si>
+    <t>Partner_Yes</t>
+  </si>
+  <si>
     <t>StreamingTV_Yes</t>
   </si>
   <si>
-    <t>Partner_Yes</t>
-  </si>
-  <si>
-    <t>MonthlyCharges</t>
+    <t>StreamingMovies_Yes</t>
+  </si>
+  <si>
+    <t>Engagement_Score</t>
   </si>
   <si>
     <t>TotalCharges</t>
   </si>
   <si>
-    <t>StreamingMovies_Yes</t>
-  </si>
-  <si>
-    <t>Engagement_Score</t>
+    <t>Dependents_Yes</t>
   </si>
   <si>
     <t>OnlineBackup_Yes</t>
   </si>
   <si>
-    <t>Dependents_Yes</t>
+    <t>Service_Utilization</t>
   </si>
   <si>
     <t>SeniorCitizen</t>
@@ -149,7 +153,7 @@
     <t>DeviceProtection_Yes</t>
   </si>
   <si>
-    <t>Service_Utilization</t>
+    <t>Payment_Reliability</t>
   </si>
   <si>
     <t>PaymentMethod_Mailed check</t>
@@ -158,36 +162,33 @@
     <t>PaymentMethod_Credit card (automatic)</t>
   </si>
   <si>
-    <t>Payment_Reliability</t>
+    <t>OnlineBackup_No internet service</t>
+  </si>
+  <si>
+    <t>PhoneService_Yes</t>
   </si>
   <si>
     <t>MultipleLines_No phone service</t>
   </si>
   <si>
+    <t>OnlineSecurity_No internet service</t>
+  </si>
+  <si>
+    <t>DeviceProtection_No internet service</t>
+  </si>
+  <si>
+    <t>StreamingTV_No internet service</t>
+  </si>
+  <si>
     <t>TechSupport_No internet service</t>
   </si>
   <si>
-    <t>PhoneService_Yes</t>
-  </si>
-  <si>
     <t>StreamingMovies_No internet service</t>
   </si>
   <si>
     <t>InternetService_No</t>
   </si>
   <si>
-    <t>OnlineBackup_No internet service</t>
-  </si>
-  <si>
-    <t>DeviceProtection_No internet service</t>
-  </si>
-  <si>
-    <t>StreamingTV_No internet service</t>
-  </si>
-  <si>
-    <t>OnlineSecurity_No internet service</t>
-  </si>
-  <si>
     <t>Best_Score</t>
   </si>
   <si>
@@ -200,7 +201,7 @@
     <t>{'n_estimators': 200, 'learning_rate': 0.1, 'max_depth': 5}</t>
   </si>
   <si>
-    <t>{'n_estimators': 389, 'learning_rate': 0.024330402377997752, 'max_depth': 9, 'subsample': 0.8530775100878596}</t>
+    <t>{'n_estimators': 264, 'learning_rate': 0.040435977764864704, 'max_depth': 8, 'subsample': 0.9396810473416601}</t>
   </si>
   <si>
     <t>{'n_estimators': 200, 'max_depth': None, 'min_samples_split': 2}</t>
@@ -218,10 +219,10 @@
     <t>{'n_estimators': 100, 'learning_rate': 1.0}</t>
   </si>
   <si>
-    <t>{'n_estimators': 329, 'learning_rate': 0.025401461056286573, 'max_depth': 10}</t>
-  </si>
-  <si>
-    <t>{'iterations': 470, 'learning_rate': 0.055830482499039276, 'depth': 8}</t>
+    <t>{'n_estimators': 337, 'learning_rate': 0.020713257301171004, 'max_depth': 9}</t>
+  </si>
+  <si>
+    <t>{'iterations': 336, 'learning_rate': 0.08491024370403978, 'depth': 10}</t>
   </si>
   <si>
     <t>Dataset_Shape</t>
@@ -257,7 +258,34 @@
     <t>(7043, 24)</t>
   </si>
   <si>
-    <t>0.29 seconds</t>
+    <t>0.31 seconds</t>
+  </si>
+  <si>
+    <t>Scenario</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>ROC_AUC</t>
+  </si>
+  <si>
+    <t>No Feature Engineering</t>
+  </si>
+  <si>
+    <t>Feature Engineering</t>
+  </si>
+  <si>
+    <t>Feature Engineering + SMOTE</t>
   </si>
 </sst>
 </file>
@@ -643,16 +671,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>0.9399862132928403</v>
+        <v>0.9408122800714469</v>
       </c>
       <c r="C2">
-        <v>0.004408357756093469</v>
+        <v>0.004439423084684349</v>
       </c>
       <c r="D2">
-        <v>0.9337781141666434</v>
+        <v>0.9352297255627505</v>
       </c>
       <c r="E2">
-        <v>0.9456174006394548</v>
+        <v>0.9474195430465122</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -660,16 +688,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>0.9399349346653103</v>
+        <v>0.9389822350837246</v>
       </c>
       <c r="C3">
-        <v>0.004154994186249861</v>
+        <v>0.003817224862165264</v>
       </c>
       <c r="D3">
-        <v>0.9336940169502612</v>
+        <v>0.9332272773993403</v>
       </c>
       <c r="E3">
-        <v>0.9451473780018202</v>
+        <v>0.9438348619571052</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -677,16 +705,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.9371586786273403</v>
+        <v>0.9365267018141573</v>
       </c>
       <c r="C4">
-        <v>0.004770549328645539</v>
+        <v>0.005620164765551236</v>
       </c>
       <c r="D4">
-        <v>0.9305216830656239</v>
+        <v>0.9287509694540222</v>
       </c>
       <c r="E4">
-        <v>0.9431912063292026</v>
+        <v>0.9435562090130458</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -694,16 +722,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.9365267018141573</v>
+        <v>0.9358021757209306</v>
       </c>
       <c r="C5">
-        <v>0.005620164765551236</v>
+        <v>0.00476923411761053</v>
       </c>
       <c r="D5">
-        <v>0.9287509694540222</v>
+        <v>0.9291677178818716</v>
       </c>
       <c r="E5">
-        <v>0.9435562090130458</v>
+        <v>0.9421326051949871</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -840,19 +868,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2">
-        <v>0.8488596830305373</v>
+        <v>0.8577502899110939</v>
       </c>
       <c r="B2">
-        <v>0.8442748091603054</v>
+        <v>0.8560431100846805</v>
       </c>
       <c r="C2">
-        <v>0.8553750966744006</v>
+        <v>0.860015467904099</v>
       </c>
       <c r="D2">
-        <v>0.8497887053399923</v>
+        <v>0.8580246913580247</v>
       </c>
       <c r="E2">
-        <v>0.9373442301968393</v>
+        <v>0.938701855550814</v>
       </c>
     </row>
   </sheetData>
@@ -881,7 +909,7 @@
         <v>22</v>
       </c>
       <c r="B2">
-        <v>0.1056053937291425</v>
+        <v>0.09831535075976734</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -889,7 +917,7 @@
         <v>23</v>
       </c>
       <c r="B3">
-        <v>0.0986179420753179</v>
+        <v>0.08452104515737395</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -897,7 +925,7 @@
         <v>24</v>
       </c>
       <c r="B4">
-        <v>0.07300695698395551</v>
+        <v>0.06505402468366005</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -905,7 +933,7 @@
         <v>25</v>
       </c>
       <c r="B5">
-        <v>0.05545561905866541</v>
+        <v>0.06423153347626288</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -913,7 +941,7 @@
         <v>26</v>
       </c>
       <c r="B6">
-        <v>0.05390967941987079</v>
+        <v>0.06207988669831658</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -921,7 +949,7 @@
         <v>27</v>
       </c>
       <c r="B7">
-        <v>0.0515911627919607</v>
+        <v>0.05524395818037838</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -929,7 +957,7 @@
         <v>28</v>
       </c>
       <c r="B8">
-        <v>0.04813526711462898</v>
+        <v>0.04605512606470746</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -937,7 +965,7 @@
         <v>29</v>
       </c>
       <c r="B9">
-        <v>0.0469590324445362</v>
+        <v>0.04476238415211353</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -945,7 +973,7 @@
         <v>30</v>
       </c>
       <c r="B10">
-        <v>0.04389220702032604</v>
+        <v>0.04283704625333935</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -953,7 +981,7 @@
         <v>31</v>
       </c>
       <c r="B11">
-        <v>0.04099343712620392</v>
+        <v>0.03879958983533133</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -961,7 +989,7 @@
         <v>32</v>
       </c>
       <c r="B12">
-        <v>0.03894688543481777</v>
+        <v>0.03842125945634847</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -969,7 +997,7 @@
         <v>33</v>
       </c>
       <c r="B13">
-        <v>0.03430473577578552</v>
+        <v>0.03838571064059735</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -977,7 +1005,7 @@
         <v>34</v>
       </c>
       <c r="B14">
-        <v>0.03414249398720823</v>
+        <v>0.03293259049817319</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -985,7 +1013,7 @@
         <v>35</v>
       </c>
       <c r="B15">
-        <v>0.03317016779921974</v>
+        <v>0.03088697596257657</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -993,7 +1021,7 @@
         <v>36</v>
       </c>
       <c r="B16">
-        <v>0.0331492231993009</v>
+        <v>0.03050738294890358</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1001,7 +1029,7 @@
         <v>37</v>
       </c>
       <c r="B17">
-        <v>0.0314018207327075</v>
+        <v>0.02984503193220509</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1009,7 +1037,7 @@
         <v>38</v>
       </c>
       <c r="B18">
-        <v>0.02935029416586906</v>
+        <v>0.02852663208842904</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1017,7 +1045,7 @@
         <v>39</v>
       </c>
       <c r="B19">
-        <v>0.02559386333463404</v>
+        <v>0.02807371620597136</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1025,7 +1053,7 @@
         <v>40</v>
       </c>
       <c r="B20">
-        <v>0.02430567990955977</v>
+        <v>0.02728885202204224</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -1033,7 +1061,7 @@
         <v>41</v>
       </c>
       <c r="B21">
-        <v>0.01870481754653981</v>
+        <v>0.01912299871012789</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -1041,7 +1069,7 @@
         <v>42</v>
       </c>
       <c r="B22">
-        <v>0.0183512915492769</v>
+        <v>0.01859785916434884</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -1049,7 +1077,7 @@
         <v>43</v>
       </c>
       <c r="B23">
-        <v>0.01583205317198501</v>
+        <v>0.01670343486910839</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -1057,7 +1085,7 @@
         <v>44</v>
       </c>
       <c r="B24">
-        <v>0.01019461334084678</v>
+        <v>0.01641862046388125</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -1065,7 +1093,7 @@
         <v>45</v>
       </c>
       <c r="B25">
-        <v>0.008214671033119635</v>
+        <v>0.01554130097768571</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -1073,7 +1101,7 @@
         <v>46</v>
       </c>
       <c r="B26">
-        <v>0.007801955749687254</v>
+        <v>0.008123237475500675</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -1081,7 +1109,7 @@
         <v>47</v>
       </c>
       <c r="B27">
-        <v>0.004477365454863085</v>
+        <v>0.005798559770640363</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -1089,7 +1117,7 @@
         <v>48</v>
       </c>
       <c r="B28">
-        <v>0.003686965305675825</v>
+        <v>0.003853627837621522</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -1097,7 +1125,7 @@
         <v>49</v>
       </c>
       <c r="B29">
-        <v>0.003343738507926415</v>
+        <v>0.003160258522460472</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -1105,7 +1133,7 @@
         <v>50</v>
       </c>
       <c r="B30">
-        <v>0.002499174218535384</v>
+        <v>0.003086195260744489</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -1113,7 +1141,7 @@
         <v>51</v>
       </c>
       <c r="B31">
-        <v>0.001522227681526917</v>
+        <v>0.002130485645282485</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -1121,7 +1149,7 @@
         <v>52</v>
       </c>
       <c r="B32">
-        <v>0.001324943316811789</v>
+        <v>0.0006953242861001574</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -1129,7 +1157,7 @@
         <v>53</v>
       </c>
       <c r="B33">
-        <v>0.0008183815607708296</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -1137,7 +1165,7 @@
         <v>54</v>
       </c>
       <c r="B34">
-        <v>0.0006959394587238863</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -1185,7 +1213,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>0.9321785069177858</v>
@@ -1199,7 +1227,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.9350274647018457</v>
+        <v>0.9351456164279991</v>
       </c>
       <c r="C4" t="s">
         <v>60</v>
@@ -1262,10 +1290,10 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>0.9343619189549616</v>
+        <v>0.9334813234350913</v>
       </c>
       <c r="C10" t="s">
         <v>66</v>
@@ -1276,7 +1304,7 @@
         <v>5</v>
       </c>
       <c r="B11">
-        <v>0.9357891764870787</v>
+        <v>0.9361114074765897</v>
       </c>
       <c r="C11" t="s">
         <v>67</v>
@@ -1338,25 +1366,118 @@
         <v>5</v>
       </c>
       <c r="D2">
-        <v>0.9399862132928403</v>
+        <v>0.9408122800714469</v>
       </c>
       <c r="E2">
-        <v>0.8488596830305373</v>
+        <v>0.8577502899110939</v>
       </c>
       <c r="F2">
-        <v>0.8442748091603054</v>
+        <v>0.8560431100846805</v>
       </c>
       <c r="G2">
-        <v>0.8553750966744006</v>
+        <v>0.860015467904099</v>
       </c>
       <c r="H2">
-        <v>0.8497887053399923</v>
+        <v>0.8580246913580247</v>
       </c>
       <c r="I2">
-        <v>0.9373442301968393</v>
+        <v>0.938701855550814</v>
       </c>
       <c r="J2" t="s">
         <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2">
+        <v>0.7847813742191937</v>
+      </c>
+      <c r="C2">
+        <v>0.6170212765957447</v>
+      </c>
+      <c r="D2">
+        <v>0.4967880085653105</v>
+      </c>
+      <c r="E2">
+        <v>0.5504151838671412</v>
+      </c>
+      <c r="F2">
+        <v>0.8248811017080976</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B3">
+        <v>0.7802385008517888</v>
+      </c>
+      <c r="C3">
+        <v>0.6104972375690608</v>
+      </c>
+      <c r="D3">
+        <v>0.4732334047109208</v>
+      </c>
+      <c r="E3">
+        <v>0.5331724969843185</v>
+      </c>
+      <c r="F3">
+        <v>0.8239866754482059</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4">
+        <v>0.8577502899110939</v>
+      </c>
+      <c r="C4">
+        <v>0.8560431100846805</v>
+      </c>
+      <c r="D4">
+        <v>0.860015467904099</v>
+      </c>
+      <c r="E4">
+        <v>0.8580246913580247</v>
+      </c>
+      <c r="F4">
+        <v>0.938701855550814</v>
       </c>
     </row>
   </sheetData>

</xml_diff>